<commit_message>
correction plan de trvail
</commit_message>
<xml_diff>
--- a/Documentation/133_GESTPROJ_GAMBERA_Luca_LEONETTI_Matteo.xlsx
+++ b/Documentation/133_GESTPROJ_GAMBERA_Luca_LEONETTI_Matteo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_DEV\133\Projet\133\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C90DD6-76DE-41E4-B318-A31F35DF2D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F812B871-5862-493D-8CA9-FA0C8175C4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
   <si>
     <t>Planning</t>
   </si>
@@ -359,6 +359,21 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Documentation TT</t>
+  </si>
+  <si>
+    <t>Réalisation des schémas</t>
+  </si>
+  <si>
+    <t>Commencement implémentation rest2</t>
+  </si>
+  <si>
+    <t>Réalisation des documents de gestion</t>
+  </si>
+  <si>
+    <t>Leonetti Matteo / Gambera Luca</t>
   </si>
 </sst>
 </file>
@@ -450,7 +465,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -498,6 +513,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -793,7 +844,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -862,18 +913,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -897,13 +952,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1247,8 +1316,8 @@
   </sheetPr>
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1433,13 +1502,13 @@
         <v>74</v>
       </c>
       <c r="H9" s="12"/>
-      <c r="I9" s="38" t="s">
+      <c r="I9" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="38" t="s">
+      <c r="J9" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="36" t="s">
+      <c r="K9" s="34" t="s">
         <v>35</v>
       </c>
       <c r="L9" s="12"/>
@@ -1458,9 +1527,9 @@
       <c r="F10" s="7"/>
       <c r="G10" s="13"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="37"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="35"/>
       <c r="L10" s="12"/>
       <c r="M10" s="7"/>
       <c r="N10" s="13"/>
@@ -1479,9 +1548,9 @@
       <c r="F11" s="7"/>
       <c r="G11" s="13"/>
       <c r="H11" s="12"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="37"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="35"/>
       <c r="L11" s="12"/>
       <c r="M11" s="7"/>
       <c r="N11" s="13"/>
@@ -1497,12 +1566,12 @@
       <c r="C12" s="7"/>
       <c r="D12" s="13"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="13"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="50"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="37"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="35"/>
       <c r="L12" s="12"/>
       <c r="M12" s="7"/>
       <c r="N12" s="13"/>
@@ -1518,12 +1587,12 @@
       <c r="C13" s="7"/>
       <c r="D13" s="13"/>
       <c r="E13" s="12"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="13"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="50"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="37"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="35"/>
       <c r="L13" s="12"/>
       <c r="M13" s="7"/>
       <c r="N13" s="13"/>
@@ -1539,12 +1608,12 @@
       <c r="C14" s="7"/>
       <c r="D14" s="13"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="13"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="50"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="37"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="35"/>
       <c r="L14" s="12"/>
       <c r="M14" s="7"/>
       <c r="N14" s="13"/>
@@ -1563,9 +1632,9 @@
       <c r="F15" s="7"/>
       <c r="G15" s="13"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="37"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="35"/>
       <c r="L15" s="12"/>
       <c r="M15" s="7"/>
       <c r="N15" s="13"/>
@@ -1582,16 +1651,16 @@
       <c r="D16" s="13"/>
       <c r="E16" s="12"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="37"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="35"/>
       <c r="L16" s="12"/>
       <c r="M16" s="7"/>
       <c r="N16" s="13"/>
       <c r="O16" s="12"/>
-      <c r="P16" s="7"/>
+      <c r="P16" s="60"/>
       <c r="Q16" s="13"/>
     </row>
     <row r="17" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1603,11 +1672,11 @@
       <c r="D17" s="13"/>
       <c r="E17" s="12"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="37"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="35"/>
       <c r="L17" s="12"/>
       <c r="M17" s="7"/>
       <c r="N17" s="13"/>
@@ -1625,10 +1694,10 @@
       <c r="E18" s="12"/>
       <c r="F18" s="7"/>
       <c r="G18" s="13"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="37"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="35"/>
       <c r="L18" s="12"/>
       <c r="M18" s="7"/>
       <c r="N18" s="13"/>
@@ -1646,12 +1715,12 @@
       <c r="E19" s="12"/>
       <c r="F19" s="7"/>
       <c r="G19" s="13"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="7"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="54"/>
       <c r="N19" s="13"/>
       <c r="O19" s="12"/>
       <c r="P19" s="7"/>
@@ -1667,10 +1736,10 @@
       <c r="E20" s="12"/>
       <c r="F20" s="7"/>
       <c r="G20" s="13"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="37"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="35"/>
       <c r="L20" s="12"/>
       <c r="M20" s="7"/>
       <c r="N20" s="13"/>
@@ -1688,10 +1757,10 @@
       <c r="E21" s="12"/>
       <c r="F21" s="7"/>
       <c r="G21" s="13"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="37"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="35"/>
       <c r="L21" s="12"/>
       <c r="M21" s="7"/>
       <c r="N21" s="13"/>
@@ -1709,10 +1778,10 @@
       <c r="E22" s="12"/>
       <c r="F22" s="7"/>
       <c r="G22" s="13"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="37"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="35"/>
       <c r="L22" s="12"/>
       <c r="M22" s="7"/>
       <c r="N22" s="13"/>
@@ -1731,10 +1800,10 @@
       <c r="F23" s="7"/>
       <c r="G23" s="13"/>
       <c r="H23" s="12"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="12"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="53"/>
       <c r="M23" s="7"/>
       <c r="N23" s="13"/>
       <c r="O23" s="12"/>
@@ -1752,10 +1821,10 @@
       <c r="F24" s="7"/>
       <c r="G24" s="13"/>
       <c r="H24" s="12"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="12"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="53"/>
       <c r="M24" s="7"/>
       <c r="N24" s="13"/>
       <c r="O24" s="12"/>
@@ -1773,10 +1842,10 @@
       <c r="F25" s="7"/>
       <c r="G25" s="13"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="12"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="55"/>
       <c r="M25" s="7"/>
       <c r="N25" s="13"/>
       <c r="O25" s="12"/>
@@ -1784,7 +1853,7 @@
       <c r="Q25" s="13"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="47" t="s">
+      <c r="A26" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B26" s="12"/>
@@ -1794,18 +1863,18 @@
       <c r="F26" s="7"/>
       <c r="G26" s="13"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="37"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="35"/>
       <c r="L26" s="12"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="12"/>
+      <c r="M26" s="62"/>
+      <c r="N26" s="61"/>
+      <c r="O26" s="55"/>
       <c r="P26" s="7"/>
       <c r="Q26" s="13"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="47" t="s">
+      <c r="A27" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B27" s="12"/>
@@ -1815,18 +1884,18 @@
       <c r="F27" s="7"/>
       <c r="G27" s="13"/>
       <c r="H27" s="12"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="37"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="35"/>
       <c r="L27" s="12"/>
       <c r="M27" s="7"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="12"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="55"/>
       <c r="P27" s="7"/>
       <c r="Q27" s="13"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="47" t="s">
+      <c r="A28" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B28" s="12"/>
@@ -1836,18 +1905,18 @@
       <c r="F28" s="7"/>
       <c r="G28" s="13"/>
       <c r="H28" s="12"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="37"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="35"/>
       <c r="L28" s="12"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="12"/>
+      <c r="M28" s="62"/>
+      <c r="N28" s="63"/>
+      <c r="O28" s="55"/>
       <c r="P28" s="7"/>
       <c r="Q28" s="13"/>
     </row>
     <row r="29" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="5" t="s">
         <v>61</v>
       </c>
       <c r="B29" s="12"/>
@@ -1857,18 +1926,18 @@
       <c r="F29" s="7"/>
       <c r="G29" s="13"/>
       <c r="H29" s="12"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="37"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="35"/>
       <c r="L29" s="12"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="12"/>
+      <c r="M29" s="62"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="55"/>
       <c r="P29" s="7"/>
       <c r="Q29" s="13"/>
     </row>
     <row r="30" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="12"/>
@@ -1878,13 +1947,13 @@
       <c r="F30" s="7"/>
       <c r="G30" s="13"/>
       <c r="H30" s="12"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="37"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="35"/>
       <c r="L30" s="12"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="12"/>
+      <c r="M30" s="62"/>
+      <c r="N30" s="63"/>
+      <c r="O30" s="55"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="13"/>
     </row>
@@ -1899,15 +1968,15 @@
       <c r="F31" s="7"/>
       <c r="G31" s="13"/>
       <c r="H31" s="12"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="37"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="35"/>
       <c r="L31" s="12"/>
       <c r="M31" s="7"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="13"/>
+      <c r="N31" s="61"/>
+      <c r="O31" s="55"/>
+      <c r="P31" s="60"/>
+      <c r="Q31" s="61"/>
     </row>
     <row r="32" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
@@ -1920,15 +1989,15 @@
       <c r="F32" s="7"/>
       <c r="G32" s="13"/>
       <c r="H32" s="12"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="37"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="35"/>
       <c r="L32" s="12"/>
       <c r="M32" s="7"/>
       <c r="N32" s="13"/>
       <c r="O32" s="12"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="13"/>
+      <c r="P32" s="60"/>
+      <c r="Q32" s="61"/>
     </row>
     <row r="33" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
@@ -1941,15 +2010,15 @@
       <c r="F33" s="7"/>
       <c r="G33" s="13"/>
       <c r="H33" s="12"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="37"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="35"/>
       <c r="L33" s="12"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="13"/>
+      <c r="M33" s="60"/>
+      <c r="N33" s="61"/>
       <c r="O33" s="12"/>
       <c r="P33" s="7"/>
-      <c r="Q33" s="13"/>
+      <c r="Q33" s="61"/>
     </row>
     <row r="34" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
@@ -1962,12 +2031,12 @@
       <c r="F34" s="30"/>
       <c r="G34" s="31"/>
       <c r="H34" s="29"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="37"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="35"/>
       <c r="L34" s="29"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="31"/>
+      <c r="M34" s="64"/>
+      <c r="N34" s="65"/>
       <c r="O34" s="29"/>
       <c r="P34" s="30"/>
       <c r="Q34" s="31"/>
@@ -1983,12 +2052,12 @@
       <c r="F35" s="30"/>
       <c r="G35" s="31"/>
       <c r="H35" s="29"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="37"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="35"/>
       <c r="L35" s="29"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="31"/>
+      <c r="M35" s="64"/>
+      <c r="N35" s="65"/>
       <c r="O35" s="29"/>
       <c r="P35" s="30"/>
       <c r="Q35" s="31"/>
@@ -2004,13 +2073,13 @@
       <c r="F36" s="30"/>
       <c r="G36" s="31"/>
       <c r="H36" s="29"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="37"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="35"/>
       <c r="L36" s="29"/>
       <c r="M36" s="30"/>
-      <c r="N36" s="31"/>
-      <c r="O36" s="29"/>
+      <c r="N36" s="57"/>
+      <c r="O36" s="59"/>
       <c r="P36" s="30"/>
       <c r="Q36" s="31"/>
     </row>
@@ -2025,13 +2094,13 @@
       <c r="F37" s="30"/>
       <c r="G37" s="31"/>
       <c r="H37" s="29"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="39"/>
-      <c r="K37" s="37"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="38"/>
+      <c r="K37" s="35"/>
       <c r="L37" s="29"/>
       <c r="M37" s="30"/>
-      <c r="N37" s="31"/>
-      <c r="O37" s="29"/>
+      <c r="N37" s="57"/>
+      <c r="O37" s="59"/>
       <c r="P37" s="30"/>
       <c r="Q37" s="31"/>
     </row>
@@ -2046,13 +2115,13 @@
       <c r="F38" s="30"/>
       <c r="G38" s="31"/>
       <c r="H38" s="29"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39"/>
-      <c r="K38" s="37"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="38"/>
+      <c r="K38" s="35"/>
       <c r="L38" s="29"/>
       <c r="M38" s="30"/>
       <c r="N38" s="31"/>
-      <c r="O38" s="29"/>
+      <c r="O38" s="59"/>
       <c r="P38" s="30"/>
       <c r="Q38" s="31"/>
     </row>
@@ -2067,13 +2136,13 @@
       <c r="F39" s="30"/>
       <c r="G39" s="31"/>
       <c r="H39" s="29"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
-      <c r="K39" s="37"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="38"/>
+      <c r="K39" s="35"/>
       <c r="L39" s="29"/>
       <c r="M39" s="30"/>
-      <c r="N39" s="31"/>
-      <c r="O39" s="29"/>
+      <c r="N39" s="57"/>
+      <c r="O39" s="59"/>
       <c r="P39" s="30"/>
       <c r="Q39" s="31"/>
     </row>
@@ -2088,13 +2157,13 @@
       <c r="F40" s="30"/>
       <c r="G40" s="31"/>
       <c r="H40" s="29"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
-      <c r="K40" s="37"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="38"/>
+      <c r="K40" s="35"/>
       <c r="L40" s="29"/>
       <c r="M40" s="30"/>
-      <c r="N40" s="31"/>
-      <c r="O40" s="29"/>
+      <c r="N40" s="57"/>
+      <c r="O40" s="59"/>
       <c r="P40" s="30"/>
       <c r="Q40" s="31"/>
     </row>
@@ -2109,13 +2178,13 @@
       <c r="F41" s="30"/>
       <c r="G41" s="31"/>
       <c r="H41" s="29"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="39"/>
-      <c r="K41" s="37"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="38"/>
+      <c r="K41" s="35"/>
       <c r="L41" s="29"/>
       <c r="M41" s="30"/>
-      <c r="N41" s="31"/>
-      <c r="O41" s="29"/>
+      <c r="N41" s="57"/>
+      <c r="O41" s="59"/>
       <c r="P41" s="30"/>
       <c r="Q41" s="31"/>
     </row>
@@ -2130,15 +2199,15 @@
       <c r="F42" s="30"/>
       <c r="G42" s="31"/>
       <c r="H42" s="29"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
-      <c r="K42" s="37"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="38"/>
+      <c r="K42" s="35"/>
       <c r="L42" s="29"/>
       <c r="M42" s="30"/>
       <c r="N42" s="31"/>
       <c r="O42" s="29"/>
-      <c r="P42" s="30"/>
-      <c r="Q42" s="31"/>
+      <c r="P42" s="58"/>
+      <c r="Q42" s="57"/>
     </row>
     <row r="43" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
@@ -2151,15 +2220,15 @@
       <c r="F43" s="30"/>
       <c r="G43" s="31"/>
       <c r="H43" s="29"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
-      <c r="K43" s="37"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="38"/>
+      <c r="K43" s="35"/>
       <c r="L43" s="29"/>
       <c r="M43" s="30"/>
       <c r="N43" s="31"/>
       <c r="O43" s="29"/>
-      <c r="P43" s="34"/>
-      <c r="Q43" s="35"/>
+      <c r="P43" s="58"/>
+      <c r="Q43" s="57"/>
     </row>
     <row r="44" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
@@ -2172,15 +2241,15 @@
       <c r="F44" s="7"/>
       <c r="G44" s="13"/>
       <c r="H44" s="12"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
-      <c r="K44" s="49"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="36"/>
       <c r="L44" s="12"/>
       <c r="M44" s="7"/>
       <c r="N44" s="13"/>
       <c r="O44" s="12"/>
       <c r="P44" s="7"/>
-      <c r="Q44" s="13"/>
+      <c r="Q44" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2214,7 +2283,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2236,14 +2305,18 @@
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="21" t="s">
+        <v>79</v>
+      </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="21"/>
+      <c r="B4" s="21" t="s">
+        <v>44</v>
+      </c>
       <c r="C4" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
@@ -2258,29 +2331,59 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="23"/>
+      <c r="A8" s="22">
+        <v>45016</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="23">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="23"/>
+      <c r="A9" s="22">
+        <v>45016</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="23">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="23"/>
+      <c r="A10" s="22">
+        <v>45016</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="23">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="23"/>
+      <c r="A11" s="22">
+        <v>45016</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="23"/>
+      <c r="A12" s="22">
+        <v>45016</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="23">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
@@ -2334,7 +2437,7 @@
       <c r="B22" s="19"/>
       <c r="C22" s="23">
         <f>SUM(C8:C21)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2390,6 +2493,62 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3fb344db-9a83-4925-8457-d4a81a8233b7" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Student_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Distribution_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <AppVersion xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Invited_Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Templates xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <CultureName xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <LMS_Mappings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Invited_Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <FolderType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <TeamsChannelId xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Math_Settings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Owner xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <NotebookType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004EEFC8B7315DA4449F69FE97A704FE57" ma:contentTypeVersion="39" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="50f196367aec8f37d0a398234b0f7b17">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cc3645a1-58b5-4da5-acb4-f681c13b5e81" xmlns:ns3="3fb344db-9a83-4925-8457-d4a81a8233b7" xmlns:ns4="52c6fd7a-766c-4f84-9f35-2a37be325271" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78bd20473fe67c3676d1740625aa318f" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="cc3645a1-58b5-4da5-acb4-f681c13b5e81"/>
@@ -2831,62 +2990,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3fb344db-9a83-4925-8457-d4a81a8233b7" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Student_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Distribution_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <AppVersion xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Invited_Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Templates xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <CultureName xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <LMS_Mappings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Invited_Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <FolderType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <TeamsChannelId xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Math_Settings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Owner xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <NotebookType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE473839-D414-4B78-82BC-08E64CD93726}">
   <ds:schemaRefs>
@@ -2896,6 +2999,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE303A41-7D70-49B7-87A8-C6207A042BC3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="52c6fd7a-766c-4f84-9f35-2a37be325271"/>
+    <ds:schemaRef ds:uri="3fb344db-9a83-4925-8457-d4a81a8233b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65228189-199F-4C24-973F-99C34CC432BB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2913,15 +3027,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE303A41-7D70-49B7-87A8-C6207A042BC3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="52c6fd7a-766c-4f84-9f35-2a37be325271"/>
-    <ds:schemaRef ds:uri="3fb344db-9a83-4925-8457-d4a81a8233b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
mise a jour planing
</commit_message>
<xml_diff>
--- a/Documentation/133_GESTPROJ_GAMBERA_Luca_LEONETTI_Matteo.xlsx
+++ b/Documentation/133_GESTPROJ_GAMBERA_Luca_LEONETTI_Matteo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_DEV\133\Projet\133\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gamer\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A6545E-91F7-46E7-A751-881FD69D504B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F2BE1E-9031-4E7A-9958-CED05338703E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="96">
   <si>
     <t>Planning</t>
   </si>
@@ -380,6 +380,48 @@
   </si>
   <si>
     <t>Implémentation rest2</t>
+  </si>
+  <si>
+    <t>27,04,2023</t>
+  </si>
+  <si>
+    <t>04,05,2023</t>
+  </si>
+  <si>
+    <t>finalisation du rest1</t>
+  </si>
+  <si>
+    <t>finalisation du rest2</t>
+  </si>
+  <si>
+    <t>Début api gateway</t>
+  </si>
+  <si>
+    <t>Début du client1</t>
+  </si>
+  <si>
+    <t>Continuation client1</t>
+  </si>
+  <si>
+    <t>Continuation api gateway</t>
+  </si>
+  <si>
+    <t>Finalisation client1</t>
+  </si>
+  <si>
+    <t>Commencement imlémentation client2</t>
+  </si>
+  <si>
+    <t>Continuation implémentation client2</t>
+  </si>
+  <si>
+    <t>Finalisation client2</t>
+  </si>
+  <si>
+    <t>Finalisation api gateway</t>
+  </si>
+  <si>
+    <t>Finalisation client</t>
   </si>
 </sst>
 </file>
@@ -1322,8 +1364,8 @@
   </sheetPr>
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="Q44" sqref="Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1779,7 +1821,9 @@
       <c r="I21" s="57"/>
       <c r="J21" s="57"/>
       <c r="K21" s="54"/>
-      <c r="L21" s="12"/>
+      <c r="L21" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="M21" s="7"/>
       <c r="N21" s="13"/>
       <c r="O21" s="12"/>
@@ -1800,7 +1844,9 @@
       <c r="I22" s="57"/>
       <c r="J22" s="57"/>
       <c r="K22" s="54"/>
-      <c r="L22" s="12"/>
+      <c r="L22" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="M22" s="7"/>
       <c r="N22" s="13"/>
       <c r="O22" s="12"/>
@@ -1821,7 +1867,9 @@
       <c r="I23" s="57"/>
       <c r="J23" s="57"/>
       <c r="K23" s="54"/>
-      <c r="L23" s="40"/>
+      <c r="L23" s="40" t="s">
+        <v>67</v>
+      </c>
       <c r="M23" s="7"/>
       <c r="N23" s="13"/>
       <c r="O23" s="12"/>
@@ -1843,7 +1891,9 @@
       <c r="J24" s="57"/>
       <c r="K24" s="54"/>
       <c r="L24" s="40"/>
-      <c r="M24" s="7"/>
+      <c r="M24" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="N24" s="13"/>
       <c r="O24" s="12"/>
       <c r="P24" s="7"/>
@@ -1885,7 +1935,9 @@
       <c r="J26" s="57"/>
       <c r="K26" s="54"/>
       <c r="L26" s="12"/>
-      <c r="M26" s="49"/>
+      <c r="M26" s="49" t="s">
+        <v>67</v>
+      </c>
       <c r="N26" s="48"/>
       <c r="O26" s="42"/>
       <c r="P26" s="7"/>
@@ -1907,7 +1959,9 @@
       <c r="K27" s="54"/>
       <c r="L27" s="12"/>
       <c r="M27" s="7"/>
-      <c r="N27" s="50"/>
+      <c r="N27" s="50" t="s">
+        <v>67</v>
+      </c>
       <c r="O27" s="42"/>
       <c r="P27" s="7"/>
       <c r="Q27" s="13"/>
@@ -1928,7 +1982,9 @@
       <c r="K28" s="54"/>
       <c r="L28" s="12"/>
       <c r="M28" s="49"/>
-      <c r="N28" s="50"/>
+      <c r="N28" s="50" t="s">
+        <v>67</v>
+      </c>
       <c r="O28" s="42"/>
       <c r="P28" s="7"/>
       <c r="Q28" s="13"/>
@@ -1948,7 +2004,9 @@
       <c r="J29" s="57"/>
       <c r="K29" s="54"/>
       <c r="L29" s="12"/>
-      <c r="M29" s="49"/>
+      <c r="M29" s="49" t="s">
+        <v>67</v>
+      </c>
       <c r="N29" s="50"/>
       <c r="O29" s="42"/>
       <c r="P29" s="7"/>
@@ -1970,7 +2028,9 @@
       <c r="K30" s="54"/>
       <c r="L30" s="12"/>
       <c r="M30" s="49"/>
-      <c r="N30" s="50"/>
+      <c r="N30" s="50" t="s">
+        <v>67</v>
+      </c>
       <c r="O30" s="42"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="13"/>
@@ -2014,7 +2074,9 @@
       <c r="K32" s="54"/>
       <c r="L32" s="12"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="13"/>
+      <c r="N32" s="13" t="s">
+        <v>67</v>
+      </c>
       <c r="O32" s="12"/>
       <c r="P32" s="47"/>
       <c r="Q32" s="48"/>
@@ -2037,7 +2099,9 @@
       <c r="K33" s="54"/>
       <c r="L33" s="12"/>
       <c r="M33" s="47"/>
-      <c r="N33" s="48"/>
+      <c r="N33" s="48" t="s">
+        <v>67</v>
+      </c>
       <c r="O33" s="12"/>
       <c r="P33" s="7"/>
       <c r="Q33" s="48"/>
@@ -2058,7 +2122,9 @@
       <c r="K34" s="54"/>
       <c r="L34" s="29"/>
       <c r="M34" s="51"/>
-      <c r="N34" s="52"/>
+      <c r="N34" s="52" t="s">
+        <v>67</v>
+      </c>
       <c r="O34" s="29"/>
       <c r="P34" s="30"/>
       <c r="Q34" s="31"/>
@@ -2079,7 +2145,9 @@
       <c r="K35" s="54"/>
       <c r="L35" s="29"/>
       <c r="M35" s="51"/>
-      <c r="N35" s="52"/>
+      <c r="N35" s="52" t="s">
+        <v>67</v>
+      </c>
       <c r="O35" s="29"/>
       <c r="P35" s="30"/>
       <c r="Q35" s="31"/>
@@ -2100,7 +2168,9 @@
       <c r="K36" s="54"/>
       <c r="L36" s="29"/>
       <c r="M36" s="30"/>
-      <c r="N36" s="44"/>
+      <c r="N36" s="44" t="s">
+        <v>67</v>
+      </c>
       <c r="O36" s="46"/>
       <c r="P36" s="30"/>
       <c r="Q36" s="31"/>
@@ -2121,7 +2191,9 @@
       <c r="K37" s="54"/>
       <c r="L37" s="29"/>
       <c r="M37" s="30"/>
-      <c r="N37" s="44"/>
+      <c r="N37" s="44" t="s">
+        <v>67</v>
+      </c>
       <c r="O37" s="46"/>
       <c r="P37" s="30"/>
       <c r="Q37" s="31"/>
@@ -2143,7 +2215,9 @@
       <c r="L38" s="29"/>
       <c r="M38" s="30"/>
       <c r="N38" s="31"/>
-      <c r="O38" s="46"/>
+      <c r="O38" s="46" t="s">
+        <v>67</v>
+      </c>
       <c r="P38" s="30"/>
       <c r="Q38" s="31"/>
     </row>
@@ -2165,7 +2239,9 @@
       <c r="M39" s="30"/>
       <c r="N39" s="44"/>
       <c r="O39" s="46"/>
-      <c r="P39" s="30"/>
+      <c r="P39" s="30" t="s">
+        <v>67</v>
+      </c>
       <c r="Q39" s="31"/>
     </row>
     <row r="40" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2186,7 +2262,9 @@
       <c r="M40" s="30"/>
       <c r="N40" s="44"/>
       <c r="O40" s="46"/>
-      <c r="P40" s="30"/>
+      <c r="P40" s="30" t="s">
+        <v>67</v>
+      </c>
       <c r="Q40" s="31"/>
     </row>
     <row r="41" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2207,7 +2285,9 @@
       <c r="M41" s="30"/>
       <c r="N41" s="44"/>
       <c r="O41" s="46"/>
-      <c r="P41" s="30"/>
+      <c r="P41" s="30" t="s">
+        <v>67</v>
+      </c>
       <c r="Q41" s="31"/>
     </row>
     <row r="42" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2228,7 +2308,9 @@
       <c r="M42" s="30"/>
       <c r="N42" s="31"/>
       <c r="O42" s="29"/>
-      <c r="P42" s="45"/>
+      <c r="P42" s="45" t="s">
+        <v>67</v>
+      </c>
       <c r="Q42" s="44"/>
     </row>
     <row r="43" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2250,7 +2332,9 @@
       <c r="N43" s="31"/>
       <c r="O43" s="29"/>
       <c r="P43" s="45"/>
-      <c r="Q43" s="44"/>
+      <c r="Q43" s="44" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="44" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
@@ -2271,7 +2355,9 @@
       <c r="N44" s="13"/>
       <c r="O44" s="12"/>
       <c r="P44" s="7"/>
-      <c r="Q44" s="43"/>
+      <c r="Q44" s="43" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2302,10 +2388,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2430,77 +2516,207 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="23"/>
+      <c r="A15" s="22">
+        <v>45029</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="23">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="23"/>
+      <c r="A16" s="22">
+        <v>45029</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="23">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="23"/>
+      <c r="A17" s="22">
+        <v>45030</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="23">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="23"/>
+      <c r="A18" s="22">
+        <v>45030</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="23">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="23"/>
+      <c r="A19" s="22">
+        <v>45030</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="23">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="23"/>
+      <c r="A20" s="22">
+        <v>45036</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="23">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="23"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
+      <c r="A21" s="22">
+        <v>45037</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="22">
+        <v>45037</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="22">
+        <v>45043</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="23">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="23">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="22">
+        <v>45044</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="22">
+        <v>45044</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="22">
+        <v>45051</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="22">
+        <v>45051</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="23">
-        <f>SUM(C8:C21)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="24" t="s">
+      <c r="B30" s="19"/>
+      <c r="C30" s="23">
+        <f>SUM(C8:C29)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="25" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="26" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="25" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="26" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="26" t="s">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="26" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2509,7 +2725,7 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="81" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LModule 133&amp;RJournal de travail</oddHeader>
     <oddFooter>&amp;C&amp;D&amp;R&amp;P/&amp;N</oddFooter>
@@ -2518,15 +2734,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004EEFC8B7315DA4449F69FE97A704FE57" ma:contentTypeVersion="39" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="50f196367aec8f37d0a398234b0f7b17">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cc3645a1-58b5-4da5-acb4-f681c13b5e81" xmlns:ns3="3fb344db-9a83-4925-8457-d4a81a8233b7" xmlns:ns4="52c6fd7a-766c-4f84-9f35-2a37be325271" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78bd20473fe67c3676d1740625aa318f" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="cc3645a1-58b5-4da5-acb4-f681c13b5e81"/>
@@ -2968,6 +3175,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3025,14 +3241,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE473839-D414-4B78-82BC-08E64CD93726}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65228189-199F-4C24-973F-99C34CC432BB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3052,6 +3260,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE473839-D414-4B78-82BC-08E64CD93726}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE303A41-7D70-49B7-87A8-C6207A042BC3}">
   <ds:schemaRefs>

</xml_diff>